<commit_message>
15 test cases are added
</commit_message>
<xml_diff>
--- a/Project_Documents/Test_cases/Test_Cases.xlsx
+++ b/Project_Documents/Test_cases/Test_Cases.xlsx
@@ -7,17 +7,203 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test Cases -  Actuators" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases -  Actuators'!$A$6:$G$6</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
+  <si>
+    <t>Test Cases ID</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>Test Case Steps</t>
+  </si>
+  <si>
+    <t>Pre-condition</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>TC_1</t>
+  </si>
+  <si>
+    <t>1. Account should be created in Tudunet
+2. Finaltest.ihex should be created.</t>
+  </si>
+  <si>
+    <t>Verify uploading ihex file on Tudunet</t>
+  </si>
+  <si>
+    <t>Responsiveness</t>
+  </si>
+  <si>
+    <t>1. Open web page "http://www.tudunet.tu-darmstadt.de/"
+2. Enter "username" and "password".
+3. Select "Jobs"
+4. Select "Manage Files"
+5. Select "Upload a file to TUDμNet"
+6. Browse "Finaltest.ihex" 
+7. Select Provide a platform type "XM1000" 
+8. Select Operating system "Contiki".
+9. Select "Upload It Now"</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>1. "Finaltest.ihex" should be uploaded</t>
+  </si>
+  <si>
+    <t>Same as Expected</t>
+  </si>
+  <si>
+    <t>TC_2</t>
+  </si>
+  <si>
+    <t>Verify creating a job on Tudunet</t>
+  </si>
+  <si>
+    <t>1. Account should be created in Tudunet
+2. Finaltest.ihex should be uploaded</t>
+  </si>
+  <si>
+    <t>1. Open web page "http://www.tudunet.tu-darmstadt.de/"
+2. Enter "username" and "password".
+3. Select "Jobs"
+4. Select "Manage Jobs"
+5. Select "Create new job"
+6. Write name "TestFianl" and description. 
+7. Click on "Next" button and Select "Finaltest.ihex" file 
+8. Click on "Next" button and  Select which program will run on individual nodes.
+9. Select "playground" nodes and click "Finish" button</t>
+  </si>
+  <si>
+    <t>1. "TestFinal" job should be created.</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t>Verify scheduling a "TestFinal" job</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as 160 for testing purpose.</t>
+  </si>
+  <si>
+    <t>TC_5</t>
+  </si>
+  <si>
+    <t>TC_6</t>
+  </si>
+  <si>
+    <t>TC_7</t>
+  </si>
+  <si>
+    <t>Verify FAN ON for both plants when C02 level is higher than Threshold Value (950 ppm)</t>
+  </si>
+  <si>
+    <t>Verify LIGHT ON for both plants when on board sensor put in shadow or Value is lower than threshold value (160)</t>
+  </si>
+  <si>
+    <t>Verify HEATER ON for both plants when soil moisture is higher than Threshold value [raw : 2428 (38.08 VWC)].</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as [raw : 2428 (38.08 VWC)] for testing purpose.</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as [raw : 1502 (10 VWC)] for testing purpose.</t>
+  </si>
+  <si>
+    <t>TC_9</t>
+  </si>
+  <si>
+    <t>TC_8</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>Verify actuators behavior when all operation peroformed at same time.</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as 29 °Cfor testing purpose.</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as 12.7 °C for testing purpose.</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>Verify FAN ON for both plants when humidity is increased than Threshold Value (40 %)</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as 40 % for testing purpose.</t>
+  </si>
+  <si>
+    <t>Verify HEATER ON for both plants when humidity is decreased than Threshold Value (20 °C)</t>
+  </si>
+  <si>
+    <t>Threshold value was taken as 20 °C for testing purpose.</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify HEATER OFF and FAN OF for both plants when humidity is between 40 % and 20% </t>
+  </si>
+  <si>
+    <t>Verify FAN OFF for both plants when temperature is lower than or equal to  Threshold Value (12.7 °C)</t>
+  </si>
+  <si>
+    <t>Verify FAN ON for both plants when temperature is higher than Threshold Value (29 °C)</t>
+  </si>
+  <si>
+    <t>Verify HEATER OFF for both plants when soil moisture is higher than or equal to Threshold value [raw : 1502 (10 VWC)]</t>
+  </si>
+  <si>
+    <t>Verify FAN OFF for both plants when C02 level is lower than or equal to Threshold Value (40 ppm)</t>
+  </si>
+  <si>
+    <t>Verify LIGHT OFF for both plants when on board sensor put in front of light or Value is higher than or equal to threshold value (160)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +211,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +247,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -55,6 +293,96 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3057525" cy="357790"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="3057525" cy="357790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Testing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Actuator functioning</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,39 +670,431 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A6:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="15.75">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="173.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="240.75" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="240">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="240">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="240">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="240">
+      <c r="A12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="240">
+      <c r="A13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="240">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="240">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="240">
+      <c r="A16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="240">
+      <c r="A17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="240">
+      <c r="A18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="240">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="240">
+      <c r="A20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="240">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A6:G6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test cases done and project report modified
</commit_message>
<xml_diff>
--- a/Project_Documents/Test_cases/Test_Cases.xlsx
+++ b/Project_Documents/Test_cases/Test_Cases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>Test Cases ID</t>
   </si>
@@ -197,29 +197,6 @@
   </si>
   <si>
     <t>Verify LIGHT OFF for both plants when on board sensor put in front of light or Value is higher than or equal to threshold value (160)</t>
-  </si>
-  <si>
-    <t>1. Account should be created in Tudunet
-2. "Finaltest.ihex" should be uploaded</t>
-  </si>
-  <si>
-    <t>1. Account should be created in Tudunet
-2. "Finaltest.ihex" should be uploaded
-3. "TestFinal" job should be created.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open web page "http://www.tudunet.tu-darmstadt.de/"
-2. Enter "username" and "password".
-3. Select "Jobs"
-4. Select "Schedule Jobs"
-5. Select "Current Date"
-6. Select "Start time" and "End Time"
-7. Select "Run - TestFinal" and "on - Playground"
-8. Select "Schedule Test".
-</t>
-  </si>
-  <si>
-    <t>1. "TestFinal" job should be scheduled and should be apper on current date.</t>
   </si>
 </sst>
 </file>
@@ -695,9 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -770,7 +745,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -786,7 +761,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="180">
+    <row r="9" spans="1:8" ht="240">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -794,13 +769,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>13</v>

</xml_diff>